<commit_message>
Added structure to backend files, connected to MySQL correctly using user nicha, and added create scripts for tables in shopping schema
</commit_message>
<xml_diff>
--- a/Data plan.xlsx
+++ b/Data plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicha\Desktop\Angular-Spring-Shopping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D51C01A6-70BB-4E52-8F97-88F91957063C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE590E8F-761B-4FC2-97DC-078CC0CF2BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5C866527-CE68-4215-8660-319350F133E0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{5C866527-CE68-4215-8660-319350F133E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>User</t>
   </si>
@@ -42,9 +42,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>role: Customer/Owner</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -60,34 +57,55 @@
     <t>status: pending/completed/failed</t>
   </si>
   <si>
-    <t>orderId</t>
-  </si>
-  <si>
     <t>OrderItem</t>
   </si>
   <si>
     <t>Product</t>
   </si>
   <si>
-    <t>productId</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>rating</t>
   </si>
   <si>
-    <t>numInStock</t>
-  </si>
-  <si>
-    <t>numSold</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>num_in_stock</t>
+  </si>
+  <si>
+    <t>num_sold</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>order[] (one user has many orders)</t>
+  </si>
+  <si>
+    <t>userId: (many orders can belong to one user)</t>
+  </si>
+  <si>
+    <t>role: Customer/Admin</t>
+  </si>
+  <si>
+    <t>total_price</t>
+  </si>
+  <si>
+    <t>total_quantity</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -112,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -163,15 +181,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C46B0C-B1DF-47CF-9FEA-336D39BF8A01}">
-  <dimension ref="C1:C29"/>
+  <dimension ref="C1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -510,28 +541,33 @@
     </row>
     <row r="4" spans="3:3">
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:3">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="3:3">
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="3:3" ht="14.65" thickBot="1"/>
     <row r="10" spans="3:3" ht="14.65" thickBot="1">
       <c r="C10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="3:3">
@@ -541,64 +577,89 @@
     </row>
     <row r="12" spans="3:3">
       <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3">
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" ht="14.65" thickBot="1"/>
+    <row r="18" spans="3:3" ht="14.65" thickBot="1">
+      <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="3:3" ht="14.65" thickBot="1"/>
-    <row r="16" spans="3:3" ht="14.65" thickBot="1">
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
-      <c r="C18" s="1" t="s">
+    <row r="19" spans="3:3">
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" ht="14.65" thickBot="1"/>
+    <row r="24" spans="3:3" ht="14.65" thickBot="1">
+      <c r="C24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="3:3" ht="14.65" thickBot="1"/>
-    <row r="22" spans="3:3" ht="14.65" thickBot="1">
-      <c r="C22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" s="2" t="s">
+    <row r="25" spans="3:3">
+      <c r="C25" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3">
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3">
-      <c r="C25" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="3:3">
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="3:3">
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>